<commit_message>
This is a long due commit after running analysis and moving things to papaja
</commit_message>
<xml_diff>
--- a/Data/Codebook.xlsx
+++ b/Data/Codebook.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>GEM NES</t>
   </si>
@@ -185,12 +185,24 @@
       <t>State of cluster development</t>
     </r>
   </si>
+  <si>
+    <t>Availability of venture capital indicates how easy it is for entrepreneurs with innovative but risky projects to find venture capital.</t>
+  </si>
+  <si>
+    <t>DOMCREDIT gap</t>
+  </si>
+  <si>
+    <t>Financial resources provided to the private sector by financial corporations as a percentage of GDP. [i]Financial resources[i] are loans, purchases of non-equity securities, and trade credits and other accounts receivable, that establish a claim for repayment.</t>
+  </si>
+  <si>
+    <t>EOSQ403: Ease of finding skilled employees</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +225,11 @@
     <font>
       <sz val="9"/>
       <name val="Calibri (body)"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -274,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -295,6 +312,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,9 +324,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +608,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -607,18 +625,18 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11"/>
+      <c r="G1" s="12"/>
       <c r="H1" s="9" t="s">
         <v>3</v>
       </c>
@@ -683,13 +701,13 @@
       <c r="B4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="8"/>
@@ -701,7 +719,7 @@
       </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" ht="26.5">
+    <row r="5" spans="1:9" s="5" customFormat="1" ht="28">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -711,7 +729,9 @@
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8" t="s">
         <v>21</v>
@@ -728,7 +748,9 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -739,7 +761,9 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="1"/>
@@ -750,7 +774,9 @@
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>

</xml_diff>